<commit_message>
clouded images filtering with value
</commit_message>
<xml_diff>
--- a/ТОО Сев. Каз СХОС/Проект смарт пастбище/Смарт п показатели 3 эксп 9.06.2022.xlsx
+++ b/ТОО Сев. Каз СХОС/Проект смарт пастбище/Смарт п показатели 3 эксп 9.06.2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Уражайность  " sheetId="1" state="visible" r:id="rId2"/>
@@ -1395,8 +1395,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2454,8 +2454,8 @@
   </sheetPr>
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5805,7 +5805,7 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -7243,14 +7243,14 @@
   </sheetPr>
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.71"/>
@@ -9295,7 +9295,7 @@
   </sheetPr>
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -12155,7 +12155,7 @@
   </sheetPr>
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B82" activeCellId="0" sqref="B82"/>
     </sheetView>
   </sheetViews>
@@ -15500,7 +15500,7 @@
   </sheetPr>
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -18783,7 +18783,7 @@
   </sheetPr>
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -20762,7 +20762,7 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>

</xml_diff>